<commit_message>
Dit is mijn commit
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Week 47" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="32">
   <si>
     <t>Logboek</t>
   </si>
@@ -105,6 +105,21 @@
   </si>
   <si>
     <t>Nieuwe game aangemaakt</t>
+  </si>
+  <si>
+    <t>Project op github gezet</t>
+  </si>
+  <si>
+    <t>Gamenaam gewijzigd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoogte en Breedte aangepast van het canvas </t>
+  </si>
+  <si>
+    <t>icoon Toegevoegd</t>
+  </si>
+  <si>
+    <t>Het spel laten stoppen en achtergrondkleur toegevoegd</t>
   </si>
 </sst>
 </file>
@@ -515,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,15 +719,21 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="C13" s="11">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0.4861111111111111</v>
+      </c>
       <c r="E13" s="1">
         <v>6</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G13" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.777777777777779E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -840,7 +861,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="14"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="1">
@@ -854,7 +875,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="14"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="1">
@@ -868,7 +889,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="14"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
       <c r="E25" s="1">
@@ -882,7 +903,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1">
@@ -896,7 +917,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1">
@@ -919,7 +940,7 @@
       </c>
       <c r="G28" s="11">
         <f>SUM(G8:G27)</f>
-        <v>0.14444444444444449</v>
+        <v>0.17222222222222228</v>
       </c>
     </row>
   </sheetData>
@@ -1362,7 +1383,7 @@
       </c>
       <c r="B7" s="5">
         <f>'Week 47'!G28</f>
-        <v>0.14444444444444449</v>
+        <v>0.17222222222222228</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1452,7 +1473,7 @@
       </c>
       <c r="B17" s="16">
         <f>SUM(B7:B16)</f>
-        <v>0.14444444444444449</v>
+        <v>0.17222222222222228</v>
       </c>
     </row>
   </sheetData>
@@ -1465,7 +1486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -1474,7 +1495,7 @@
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" customWidth="1"/>
+    <col min="6" max="6" width="52.85546875" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1546,58 +1567,84 @@
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="B8" s="10">
+        <v>41603</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.49027777777777781</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0.50069444444444444</v>
+      </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G8" s="11">
         <f>D8-C8</f>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="C9" s="11">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0.51111111111111118</v>
+      </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="G9" s="11">
         <f t="shared" ref="G9:G21" si="0">D9-C9</f>
-        <v>0</v>
+        <v>1.0416666666666741E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="C10" s="11">
+        <v>0.51111111111111118</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0.5180555555555556</v>
+      </c>
       <c r="E10" s="1">
         <v>3</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="G10" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444198E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="C11" s="11">
+        <v>0.51874999999999993</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0.53125</v>
+      </c>
       <c r="E11" s="1">
         <v>4</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G11" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.2500000000000067E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3286,7 +3333,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Nieuwe  mappen Game en GameScenes gemaakt, class StartScene gemaakt
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="36">
   <si>
     <t>Logboek</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>Het spel laten stoppen en achtergrondkleur toegevoegd</t>
+  </si>
+  <si>
+    <t>Wijzingen op GitHub gezet</t>
+  </si>
+  <si>
+    <t>Nieuwe mapjes gemaakt voor GameScenes</t>
+  </si>
+  <si>
+    <t>Aanpassingen gemaakt aan class StartScene</t>
+  </si>
+  <si>
+    <t>Laatste commit gemaakt.</t>
   </si>
 </sst>
 </file>
@@ -531,7 +543,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D13"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,7 +1404,7 @@
       </c>
       <c r="B8" s="5">
         <f>'Week 48'!G28</f>
-        <v>0</v>
+        <v>7.8472222222222276E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1473,7 +1485,7 @@
       </c>
       <c r="B17" s="16">
         <f>SUM(B7:B16)</f>
-        <v>0.17222222222222228</v>
+        <v>0.25069444444444455</v>
       </c>
     </row>
   </sheetData>
@@ -1650,57 +1662,81 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="C12" s="11">
+        <v>0.5625</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0.57291666666666663</v>
+      </c>
       <c r="E12" s="1">
         <v>5</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="G12" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.041666666666663E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
+      <c r="C13" s="11">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0.58680555555555558</v>
+      </c>
       <c r="E13" s="1">
         <v>6</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="G13" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3888888888888951E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="C14" s="11">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0.59375</v>
+      </c>
       <c r="E14" s="1">
         <v>7</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G14" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444198E-3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
+      <c r="C15" s="11">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0.61111111111111105</v>
+      </c>
       <c r="E15" s="1">
         <v>8</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="G15" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444198E-3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1863,7 +1899,8 @@
         <v>17</v>
       </c>
       <c r="G28" s="11">
-        <v>0</v>
+        <f>SUM(G8:G27)</f>
+        <v>7.8472222222222276E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nieuwe classe HelperClass gemaakt
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Week 47" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="49">
   <si>
     <t>Logboek</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>Lokale commit gemaakt</t>
+  </si>
+  <si>
+    <t>Maandag</t>
+  </si>
+  <si>
+    <t>Nieuwe map HelperScene gemaakt, using, namespace en class in public veranderd</t>
+  </si>
+  <si>
+    <t>Game opgestart en logboek bijgewerkt. Nieuwe map gemaakt in Content voor de afbeeldingen</t>
   </si>
 </sst>
 </file>
@@ -245,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -274,6 +283,30 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1436,7 +1469,7 @@
       </c>
       <c r="B10" s="5">
         <f>'Week 50'!G28</f>
-        <v>0</v>
+        <v>2.2916666666666696E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1499,7 +1532,7 @@
       </c>
       <c r="B17" s="16">
         <f>SUM(B7:B16)</f>
-        <v>0.4256944444444446</v>
+        <v>0.44861111111111129</v>
       </c>
     </row>
   </sheetData>
@@ -1945,8 +1978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2391,8 +2424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,278 +2491,307 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="1">
+    <row r="8" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="20">
+        <v>41617</v>
+      </c>
+      <c r="C8" s="21">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D8" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="E8" s="19">
         <v>1</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="1">
+      <c r="F8" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="21">
+        <f>D8-C8</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="D9" s="21">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="E9" s="19">
         <v>2</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="11">
-        <f t="shared" ref="G9:G21" si="0">D9-C9</f>
-        <v>0</v>
+      <c r="F9" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="21">
+        <f t="shared" ref="G9:G26" si="0">D9-C9</f>
+        <v>1.2500000000000011E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="1">
+      <c r="A10" s="19"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="19">
         <v>3</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="11">
+      <c r="F10" s="22"/>
+      <c r="G10" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="1">
+      <c r="A11" s="19"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="19">
         <v>4</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="11">
+      <c r="F11" s="22"/>
+      <c r="G11" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="1">
+      <c r="A12" s="19"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="19">
         <v>5</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="11">
+      <c r="F12" s="22"/>
+      <c r="G12" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="1">
+      <c r="A13" s="19"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="19">
         <v>6</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="11">
+      <c r="F13" s="22"/>
+      <c r="G13" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="1">
+      <c r="A14" s="19"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="19">
         <v>7</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="11">
+      <c r="F14" s="22"/>
+      <c r="G14" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="1">
+      <c r="A15" s="19"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="19">
         <v>8</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="11">
+      <c r="F15" s="22"/>
+      <c r="G15" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="1">
+      <c r="A16" s="19"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="19">
         <v>9</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="11">
+      <c r="F16" s="22"/>
+      <c r="G16" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="1">
+      <c r="A17" s="19"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="19">
         <v>10</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="11">
+      <c r="F17" s="22"/>
+      <c r="G17" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="1">
+      <c r="A18" s="19"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="19">
         <v>11</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="11">
+      <c r="F18" s="22"/>
+      <c r="G18" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="1">
+      <c r="A19" s="19"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="19">
         <v>12</v>
       </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="11">
+      <c r="F19" s="22"/>
+      <c r="G19" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="1">
+      <c r="A20" s="19"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="19">
         <v>13</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="11">
+      <c r="F20" s="22"/>
+      <c r="G20" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="1">
+      <c r="A21" s="19"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="19">
         <v>14</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="11">
+      <c r="F21" s="22"/>
+      <c r="G21" s="21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="7" t="s">
+      <c r="A22" s="19"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="11"/>
+      <c r="G22" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="1">
+      <c r="A23" s="19"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="19">
         <v>10</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="1">
+      <c r="A24" s="19"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="19">
         <v>11</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="1">
+      <c r="A25" s="19"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="19">
         <v>12</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19">
         <v>13</v>
       </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19">
         <v>14</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="21">
+        <f>D27-C27</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -2740,9 +2802,9 @@
       <c r="F28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="21">
         <f>SUM(G8:G27)</f>
-        <v>0</v>
+        <v>2.2916666666666696E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
/ Deze if - instructie checked of er op de rechterpijltoets wordt gedrukt.
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="58">
   <si>
     <t>Logboek</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>Image toegevoegd voor start, load, help, scores en quit en gedefineerd in de fields en in de draw methode</t>
+  </si>
+  <si>
+    <t>Variabele buttonActive gedefineerd en de switch case gedefineerd en break.</t>
+  </si>
+  <si>
+    <t>Commit gemaakt en gepushed</t>
   </si>
 </sst>
 </file>
@@ -1490,7 +1496,7 @@
       </c>
       <c r="B10" s="5">
         <f>'Week 50'!G28</f>
-        <v>9.5833333333333381E-2</v>
+        <v>0.12708333333333333</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1553,7 +1559,7 @@
       </c>
       <c r="B17" s="16">
         <f>SUM(B7:B16)</f>
-        <v>0.52152777777777803</v>
+        <v>0.55277777777777792</v>
       </c>
     </row>
   </sheetData>
@@ -2445,8 +2451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2702,32 +2708,44 @@
         <v>3.4722222222222654E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
+      <c r="C17" s="21">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D17" s="21">
+        <v>0.50902777777777775</v>
+      </c>
       <c r="E17" s="19">
         <v>10</v>
       </c>
-      <c r="F17" s="22"/>
+      <c r="F17" s="22" t="s">
+        <v>56</v>
+      </c>
       <c r="G17" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.9861111111111061E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
+      <c r="C18" s="21">
+        <v>0.50902777777777775</v>
+      </c>
+      <c r="D18" s="21">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E18" s="19">
         <v>11</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="F18" s="22" t="s">
+        <v>57</v>
+      </c>
       <c r="G18" s="21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.388888888888884E-3</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2867,7 +2885,7 @@
       </c>
       <c r="G28" s="21">
         <f>SUM(G8:G27)</f>
-        <v>9.5833333333333381E-2</v>
+        <v>0.12708333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Input edgedetectkeydown gemaakt om van scenes te veranderen
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Week 47" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="62">
   <si>
     <t>Logboek</t>
   </si>
@@ -198,6 +198,18 @@
   </si>
   <si>
     <t>Commit gemaakt en gepushed</t>
+  </si>
+  <si>
+    <t>Format logboek bijgewerkt mapje          week 51 gemaakt. Game opgestart en gestest of hij het nog deed</t>
+  </si>
+  <si>
+    <t>code verkort door een helper in de menu scene te zetten</t>
+  </si>
+  <si>
+    <t>Input.EdgeDetectKeyDown gemaakt zodat je van startscene naar playscene kan en ook terug</t>
+  </si>
+  <si>
+    <t>commit gemaakt</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1517,7 @@
       </c>
       <c r="B11" s="5">
         <f>'Week 51'!G28</f>
-        <v>0</v>
+        <v>3.819444444444442E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1559,7 +1571,7 @@
       </c>
       <c r="B17" s="16">
         <f>SUM(B7:B16)</f>
-        <v>0.55277777777777792</v>
+        <v>0.59097222222222234</v>
       </c>
     </row>
   </sheetData>
@@ -2451,7 +2463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -2898,12 +2910,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="5" max="5" width="4" customWidth="1"/>
@@ -2975,268 +2988,309 @@
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="20">
+        <v>41624</v>
+      </c>
+      <c r="C8" s="21">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D8" s="21">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="E8" s="19">
+        <v>1</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="11">
+        <f>D8-C8</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="21">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="D9" s="21">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="E9" s="19">
+        <v>2</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" ref="G9:G27" si="0">D9-C9</f>
+        <v>1.0416666666666685E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="21">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D10" s="21">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="E10" s="19">
+        <v>3</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="19">
+        <v>4</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="19">
+        <v>5</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="19">
+        <v>6</v>
+      </c>
+      <c r="F13" s="22"/>
+      <c r="G13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="19">
+        <v>7</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="19">
+        <v>8</v>
+      </c>
+      <c r="F15" s="22"/>
+      <c r="G15" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="19">
+        <v>9</v>
+      </c>
+      <c r="F16" s="22"/>
+      <c r="G16" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="19">
+        <v>10</v>
+      </c>
+      <c r="F17" s="22"/>
+      <c r="G17" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="19">
+        <v>11</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="19">
+        <v>12</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="19">
+        <v>13</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="19">
+        <v>14</v>
+      </c>
+      <c r="F21" s="22"/>
+      <c r="G21" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="19">
         <v>15</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="1">
-        <v>2</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="11">
-        <f t="shared" ref="G9:G21" si="0">D9-C9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="1">
-        <v>3</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="1">
-        <v>4</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="1">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="1">
-        <v>6</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="1">
-        <v>7</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="1">
-        <v>8</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="1">
-        <v>9</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="1">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="1">
-        <v>11</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="1">
-        <v>12</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="1">
-        <v>13</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="1">
-        <v>14</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="11"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="1">
-        <v>10</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="19">
+        <v>16</v>
+      </c>
+      <c r="F23" s="22"/>
+      <c r="G23" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="1">
-        <v>11</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="19">
+        <v>17</v>
+      </c>
+      <c r="F24" s="22"/>
+      <c r="G24" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="1">
-        <v>12</v>
-      </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="19">
+        <v>18</v>
+      </c>
+      <c r="F25" s="22"/>
+      <c r="G25" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1">
-        <v>13</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19">
+        <v>19</v>
+      </c>
+      <c r="F26" s="22"/>
+      <c r="G26" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1">
-        <v>14</v>
-      </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19">
+        <v>20</v>
+      </c>
+      <c r="F27" s="19"/>
+      <c r="G27" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -3249,7 +3303,7 @@
       </c>
       <c r="G28" s="11">
         <f>SUM(G8:G27)</f>
-        <v>0</v>
+        <v>3.819444444444442E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Draaipunt verandert van de Draw method in AnimatedSprite class
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" firstSheet="2" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Week 47" sheetId="1" r:id="rId1"/>
@@ -17,15 +17,17 @@
     <sheet name="Week 2" sheetId="10" r:id="rId8"/>
     <sheet name="Week 3" sheetId="11" r:id="rId9"/>
     <sheet name="Week 4" sheetId="12" r:id="rId10"/>
-    <sheet name="Totaal" sheetId="2" r:id="rId11"/>
-    <sheet name="toets 1 GameScene" sheetId="13" r:id="rId12"/>
+    <sheet name="week 5" sheetId="14" r:id="rId11"/>
+    <sheet name="Totaal" sheetId="2" r:id="rId12"/>
+    <sheet name="toets 1 GameScene" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet3" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="117">
   <si>
     <t>Logboek</t>
   </si>
@@ -358,6 +360,24 @@
   </si>
   <si>
     <t>ExplorerIdle aangepast</t>
+  </si>
+  <si>
+    <t>Maak in de AnimatedSprite class een field: private Vector2 pivot</t>
+  </si>
+  <si>
+    <t>Geef this.pivot in de constructor van de AnimatedSprite class de waarde new Vector2(16f, 16)</t>
+  </si>
+  <si>
+    <t>Verander in de Draw method in de AnimatedSprite class het argument origin van Vector2.Zero naar this.pivot</t>
+  </si>
+  <si>
+    <t>Verander de grenswaarden van de omkeerpunten van de beetles zodat ze niet buiten het scherm komen en niet eerder omkeren.</t>
+  </si>
+  <si>
+    <t>Verander de grenswaarden van de omkeerpunten van de scorpions zodat ze niet buiten het scherm komen en niet eerder omkeren.</t>
+  </si>
+  <si>
+    <t>Maak een commit genaamd: "Draaipunt verandert van de Draw method in AnimatedSprite class"</t>
   </si>
 </sst>
 </file>
@@ -465,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -569,6 +589,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1274,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,10 +1737,392 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="10">
+        <v>41666</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="11">
+        <f>D8-C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="11">
+        <f t="shared" ref="G9:G21" si="0">D9-C9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="1">
+        <v>6</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="1">
+        <v>7</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="1">
+        <v>8</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="1">
+        <v>9</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="1">
+        <v>10</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="1">
+        <v>11</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="1">
+        <v>12</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="1">
+        <v>13</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="1">
+        <v>14</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="1">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="11">
+        <f>D23-C23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="1">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="11">
+        <f t="shared" ref="G24:G27" si="1">D24-C24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="1">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="1">
+        <v>13</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="1">
+        <v>14</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="11">
+        <f>SUM(G8:G27)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,11 +2258,20 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="16">
-        <f>SUM(B7:B16)</f>
+      <c r="A17" s="15">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5">
+        <f>'week 5'!G28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="16">
+        <f>SUM(B7:B17)</f>
         <v>0.7743055555555558</v>
       </c>
     </row>
@@ -1867,7 +2281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
@@ -2187,6 +2601,256 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="32">
+        <v>41666</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="E7" s="31">
+        <v>1</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="33">
+        <f t="shared" ref="G7:G14" si="0">D7-C7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="33">
+        <v>0.38472222222222219</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="E8" s="31">
+        <v>2</v>
+      </c>
+      <c r="F8" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="33">
+        <f t="shared" si="0"/>
+        <v>6.9444444444449749E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="33">
+        <v>0.38611111111111113</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0.38680555555555557</v>
+      </c>
+      <c r="E9" s="31">
+        <v>3</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="G9" s="33">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="33">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0.38819444444444445</v>
+      </c>
+      <c r="E10" s="31">
+        <v>4</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="33">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="33">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="E11" s="31">
+        <v>5</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="G11" s="33">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222099E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="33">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0.39374999999999999</v>
+      </c>
+      <c r="E12" s="31">
+        <v>6</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="33">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="31"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="31">
+        <v>7</v>
+      </c>
+      <c r="F13" s="34"/>
+      <c r="G13" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="31">
+        <v>8</v>
+      </c>
+      <c r="F14" s="34"/>
+      <c r="G14" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="33">
+        <f>SUM(G7:G14)</f>
+        <v>6.9444444444444753E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
explorer kan omhoog lopen
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" firstSheet="3" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Week 47" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,15 @@
     <sheet name="week 5" sheetId="14" r:id="rId11"/>
     <sheet name="Totaal" sheetId="2" r:id="rId12"/>
     <sheet name="toets 1 GameScene" sheetId="13" r:id="rId13"/>
-    <sheet name="Sheet3" sheetId="16" r:id="rId14"/>
+    <sheet name="Toets 2" sheetId="16" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId15"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="134">
   <si>
     <t>Logboek</t>
   </si>
@@ -396,6 +397,39 @@
   </si>
   <si>
     <t>update method veranderd van explorerwalkdown en left en right.</t>
+  </si>
+  <si>
+    <t>Toets 3 States</t>
+  </si>
+  <si>
+    <t>Opdracht: zorg ervoor dat de explorer omhoog kan lopen met de juiste orientatie</t>
+  </si>
+  <si>
+    <t>Maak een copy van de ExplorerWalkDown class en hernoem deze naar ExplorerWalkUp</t>
+  </si>
+  <si>
+    <t>Verander in  ExplorerWalkUp.cs de class naam naar ExplorerWalkUp en verander ook de constructornaam naar ExplorerWalkUp</t>
+  </si>
+  <si>
+    <t>Maak in de Explorer class een field private ExplorerWalkUp walkUp, een get-property voor dit field</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zet in de constructor van de ExplorerWalkUp class een nieuw this.walkUp = new ExplorerWalkUp(this) .</t>
+  </si>
+  <si>
+    <t>Voeg aan de Update method van de ExplorerIdle class inputdetectioncode om de explorer in de walkUp toestand te kunnen brengen</t>
+  </si>
+  <si>
+    <t>Verander in de Update method van de  ExplorerWalkUp class this.explorer.Position zodat de explorer naar boven loopt.</t>
+  </si>
+  <si>
+    <t>Verander in de constructor van de ExplorerWalkUp class de rotation (denk aan -(float)Math.Pi/2, een draaiing tegen de klok in) en het effect om de orientatie goed te krijgen van je explorer. Terwijl hij omhoog loopt</t>
+  </si>
+  <si>
+    <t>Test of de explorer omhoog kan lopen met de juiste orientatie (gezicht omhoog)</t>
+  </si>
+  <si>
+    <t>Maak een commit -m: "Explorer kan omhoog lopen"</t>
   </si>
 </sst>
 </file>
@@ -503,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -610,6 +644,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1757,7 +1794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -2926,6 +2963,290 @@
       <c r="E16" s="36"/>
       <c r="F16" s="39"/>
       <c r="G16" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="32">
+        <v>41666</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0.5708333333333333</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0.5708333333333333</v>
+      </c>
+      <c r="E7" s="31">
+        <v>1</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="33">
+        <f t="shared" ref="G7:G15" si="0">D7-C7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="33">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="E8" s="31">
+        <v>2</v>
+      </c>
+      <c r="F8" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="33">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0.57222222222222219</v>
+      </c>
+      <c r="E9" s="31">
+        <v>3</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" s="33">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="33">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="E10" s="31">
+        <v>4</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="33">
+        <f t="shared" si="0"/>
+        <v>2.083333333333437E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="33">
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0.5756944444444444</v>
+      </c>
+      <c r="E11" s="31">
+        <v>5</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="33">
+        <f t="shared" si="0"/>
+        <v>6.9444444444433095E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="33">
+        <v>0.5756944444444444</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="E12" s="31">
+        <v>6</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="33">
+        <f t="shared" si="0"/>
+        <v>6.94444444444553E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="31"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="33">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="E13" s="31">
+        <v>7</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="33">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="33">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0.59236111111111112</v>
+      </c>
+      <c r="E14" s="31">
+        <v>8</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="33">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333259E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="33">
+        <v>0.59236111111111112</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0.59305555555555556</v>
+      </c>
+      <c r="E15" s="31">
+        <v>9</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="33">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="33">
+        <f>SUM(G7:G15)</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
steentjes op het scherm
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" firstSheet="3" activeTab="15"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Week 47" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,19 @@
     <sheet name="Week 3" sheetId="11" r:id="rId9"/>
     <sheet name="Week 4" sheetId="12" r:id="rId10"/>
     <sheet name="week 5" sheetId="14" r:id="rId11"/>
-    <sheet name="Totaal" sheetId="2" r:id="rId12"/>
-    <sheet name="Toets 1" sheetId="13" r:id="rId13"/>
-    <sheet name="Toets 2" sheetId="16" r:id="rId14"/>
-    <sheet name="Toets 3" sheetId="17" r:id="rId15"/>
-    <sheet name="Toets 4" sheetId="18" r:id="rId16"/>
+    <sheet name="week 6" sheetId="19" r:id="rId12"/>
+    <sheet name="Totaal" sheetId="2" r:id="rId13"/>
+    <sheet name="Toets 1" sheetId="13" r:id="rId14"/>
+    <sheet name="Toets 2" sheetId="16" r:id="rId15"/>
+    <sheet name="Toets 3" sheetId="17" r:id="rId16"/>
+    <sheet name="Toets 4" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="145">
   <si>
     <t>Logboek</t>
   </si>
@@ -449,6 +450,21 @@
   </si>
   <si>
     <t>Maak een commit -m "Explorer kan niet meer uit het scherm lopen"</t>
+  </si>
+  <si>
+    <t>game opgestart, format logboek gewijzigd</t>
+  </si>
+  <si>
+    <t>nieuwe textbestand gemaakt in content</t>
+  </si>
+  <si>
+    <t>de waarde x 20 en y 15 ingevoerd met x</t>
+  </si>
+  <si>
+    <t>nieuwe folder gemaakt level en als nieuwe classe</t>
+  </si>
+  <si>
+    <t>In de levelclass nieuwe fields gemaakt en properties en de constructor gemaakt</t>
   </si>
 </sst>
 </file>
@@ -2253,6 +2269,424 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="10">
+        <v>41666</v>
+      </c>
+      <c r="C8" s="44">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D8" s="44">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" s="11">
+        <f>D8-C8</f>
+        <v>3.4722222222221544E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="44">
+        <v>0.375</v>
+      </c>
+      <c r="D9" s="44">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" ref="G9:G21" si="0">D9-C9</f>
+        <v>5.5555555555555358E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="44">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="D10" s="44">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="44">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D11" s="44">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="11">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333814E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="44">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="D12" s="44">
+        <v>0.38472222222222219</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="11">
+        <f t="shared" si="0"/>
+        <v>6.9444444444438647E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="44">
+        <v>0.38472222222222219</v>
+      </c>
+      <c r="D13" s="44">
+        <v>0.39097222222222222</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G13" s="11">
+        <f t="shared" si="0"/>
+        <v>6.2500000000000333E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="1">
+        <v>7</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="1">
+        <v>8</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="1">
+        <v>9</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="1">
+        <v>10</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="1">
+        <v>11</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="1">
+        <v>12</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="1">
+        <v>13</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="1">
+        <v>14</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="1">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="11">
+        <f>D23-C23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="1">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="11">
+        <f t="shared" ref="G24:G27" si="1">D24-C24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="1">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="1">
+        <v>13</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="1">
+        <v>14</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="11">
+        <f>SUM(G8:G27)</f>
+        <v>1.9444444444444375E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -2415,7 +2849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
@@ -2738,7 +3172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -2988,7 +3422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
@@ -3272,11 +3706,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -3412,11 +3846,11 @@
       <c r="A10" s="31"/>
       <c r="B10" s="32"/>
       <c r="C10" s="33">
-        <f t="shared" ref="C8:C14" si="1">D9+TIME(0,1,0)</f>
+        <f t="shared" ref="C10" si="1">D9+TIME(0,1,0)</f>
         <v>0.59861111111111109</v>
       </c>
       <c r="D10" s="33">
-        <f t="shared" ref="D7:D14" si="2">C10+TIME(0,1,0)</f>
+        <f t="shared" ref="D10" si="2">C10+TIME(0,1,0)</f>
         <v>0.59930555555555554</v>
       </c>
       <c r="E10" s="31">

</xml_diff>